<commit_message>
Begin of tests, fix bounds, works
</commit_message>
<xml_diff>
--- a/tests/data/Tests.xlsx
+++ b/tests/data/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\god79\source\repos\LR1\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C3C707-CF4F-4B2A-B90F-98D991B1404E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4FE6D1-5CBA-4AFA-AA43-286DE409CE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,7 +124,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,16 +135,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -149,12 +165,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -437,1519 +491,2950 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B209" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:R241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="62.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
       <c r="B1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" s="3"/>
       <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G1" s="4"/>
       <c r="H1" t="s">
         <v>8</v>
       </c>
+      <c r="I1" s="3"/>
       <c r="J1" t="s">
         <v>11</v>
       </c>
+      <c r="K1" s="3"/>
       <c r="L1" t="s">
         <v>12</v>
       </c>
+      <c r="M1" s="3"/>
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="3"/>
       <c r="P1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="3"/>
       <c r="R1" t="s">
         <v>15</v>
       </c>
+      <c r="S1" s="3"/>
       <c r="T1" t="s">
         <v>16</v>
       </c>
+      <c r="U1" s="3"/>
       <c r="V1" t="s">
         <v>9</v>
       </c>
+      <c r="W1" s="3"/>
       <c r="X1" t="s">
         <v>17</v>
       </c>
+      <c r="Y1" s="3"/>
       <c r="Z1" t="s">
         <v>18</v>
       </c>
+      <c r="AA1" s="3"/>
       <c r="AB1" t="s">
         <v>19</v>
       </c>
+      <c r="AC1" s="3"/>
       <c r="AD1" t="s">
         <v>20</v>
       </c>
+      <c r="AE1" s="3"/>
       <c r="AF1" t="s">
         <v>21</v>
       </c>
+      <c r="AG1" s="3"/>
       <c r="AH1" t="s">
         <v>22</v>
       </c>
+      <c r="AI1" s="3"/>
       <c r="AJ1" t="s">
         <v>10</v>
       </c>
+      <c r="AK1" s="3"/>
       <c r="AL1" t="s">
         <v>23</v>
       </c>
+      <c r="AM1" s="3"/>
       <c r="AN1" t="s">
         <v>24</v>
       </c>
+      <c r="AO1" s="3"/>
       <c r="AP1" t="s">
         <v>25</v>
       </c>
+      <c r="AQ1" s="3"/>
       <c r="AR1" t="s">
         <v>26</v>
       </c>
+      <c r="AS1" s="3"/>
       <c r="AT1" t="s">
         <v>27</v>
       </c>
+      <c r="AU1" s="3"/>
       <c r="AV1" t="s">
         <v>28</v>
       </c>
+      <c r="AW1" s="3"/>
       <c r="AX1" t="s">
         <v>29</v>
       </c>
+      <c r="AY1" s="3"/>
       <c r="AZ1" t="s">
         <v>30</v>
       </c>
+      <c r="BA1" s="3"/>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AI2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AK2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AL2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AM2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AN2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AO2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AP2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AR2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AS2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AT2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AU2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AV2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AW2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AX2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AY2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BA2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AQ3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AW3" s="3"/>
+      <c r="AY3" s="3"/>
+      <c r="BA3" s="3"/>
+    </row>
+    <row r="4" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+      <c r="S4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AW4" s="3"/>
+      <c r="AY4" s="3"/>
+      <c r="BA4" s="3"/>
+    </row>
+    <row r="5" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AU5" s="3"/>
+      <c r="AW5" s="3"/>
+      <c r="AY5" s="3"/>
+      <c r="BA5" s="3"/>
+    </row>
+    <row r="6" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="I6" s="2"/>
+      <c r="P6" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R6" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P7" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R7" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P8" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R8" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P9" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R9" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P10" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R10" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P11" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R11" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P12" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R12" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P13" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R13" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P14" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R14" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="P15" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R15" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P16" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R16" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P17" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R17" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P18" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R18" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P19" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R19" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P20" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R20" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P21" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R21" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P22" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R22" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P23" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R23" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P24" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R24" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P25" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R25" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P26" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R26" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P27" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R27" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P28" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R28" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P29" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R29" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P30" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R30" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P31" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R31" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P32" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R32" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P33" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R33" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P34" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R34" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P35" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R35" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P36" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R36" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P37" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R37" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P38" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R38" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P39" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R39" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P40" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R40" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P41" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R41" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P42" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R42" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P43" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R43" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P44" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R44" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P45" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R45" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P46" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R46" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P47" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R47" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P48" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R48" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P49" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R49" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P50" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R50" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P51" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R51" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P52" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R52" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P53" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R53" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P54" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R54" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P55" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R55" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P56" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R56" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P57" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R57" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P58" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R58" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P59" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R59" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P60" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R60" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P61" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R61" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P62" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R62" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P63" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R63" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P64" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R64" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P65" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R65" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P66" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R66" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P67" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R67" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P68" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R68" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P69" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R69" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P70" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R70" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P71" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R71" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P72" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R72" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P73" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R73" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P74" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R74" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P75" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R75" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P76" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R76" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P77" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R77" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P78" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R78" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P79" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R79" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P80" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R80" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P81" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R81" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P82" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R82" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P83" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R83" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P84" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R84" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P85" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R85" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P86" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R86" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P87" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R87" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P88" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R88" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P89" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R89" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P90" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R90" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P91" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R91" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P92" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R92" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P93" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R93" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P94" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R94" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P95" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R95" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P96" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R96" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P97" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R97" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P98" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R98" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P99" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R99" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P100" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R100" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P101" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R101" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P102" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R102" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P103" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R103" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P104" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R104" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P105" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R105" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P106" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R106" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P107" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R107" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P108" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R108" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P109" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R109" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P110" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R110" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P111" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R111" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P112" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R112" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P113" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R113" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P114" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R114" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P115" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R115" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P116" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R116" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P117" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R117" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P118" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R118" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P119" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R119" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P120" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R120" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P121" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R121" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P122" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R122" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P123" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R123" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P124" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R124" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P125" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R125" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P126" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R126" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P127" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R127" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P128" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R128" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P129" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R129" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P130" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R130" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P131" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R131" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P132" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R132" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P133" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R133" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P134" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R134" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P135" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R135" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P136" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R136" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P137" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R137" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P138" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R138" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P139" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R139" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P140" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R140" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P141" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R141" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P142" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R142" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P143" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R143" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P144" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R144" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P145" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R145" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>144</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P146" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R146" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P147" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R147" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>146</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P148" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R148" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P149" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R149" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>148</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P150" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R150" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P151" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R151" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>150</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P152" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R152" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P153" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R153" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>152</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P154" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R154" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P155" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R155" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>154</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P156" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R156" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P157" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R157" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>156</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P158" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R158" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P159" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R159" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>158</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P160" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R160" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P161" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R161" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>160</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P162" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R162" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P163" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R163" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P164" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R164" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P165" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R165" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>164</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P166" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R166" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P167" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R167" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>166</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P168" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R168" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P169" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R169" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>168</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P170" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R170" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P171" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R171" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>170</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P172" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R172" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P173" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R173" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>172</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P174" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R174" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P175" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R175" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P176" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R176" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P177" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R177" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P178" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R178" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P179" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R179" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P180" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R180" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P181" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R181" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P182" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R182" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P183" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R183" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P184" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R184" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P185" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R185" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="186" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>184</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P186" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R186" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P187" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R187" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P188" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R188" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P189" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R189" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P190" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R190" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P191" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R191" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P192" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R192" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="193" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P193" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R193" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>192</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P194" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R194" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="195" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P195" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R195" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="196" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>194</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P196" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R196" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="197" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P197" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R197" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>196</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P198" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R198" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P199" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R199" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>198</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P200" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R200" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="201" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P201" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R201" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="202" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>200</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P202" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R202" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="P203" s="9">
+        <v>-3.4028234699999998E+38</v>
+      </c>
+      <c r="R203" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>202</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R204" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R205" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R206" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="207" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R207" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>206</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R208" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="209" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R209" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="210" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R210" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="211" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R211" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="212" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R212" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="213" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R213" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="214" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>212</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R214" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="215" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R215" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="216" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R216" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="217" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R217" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="218" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>216</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R218" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="219" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R219" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="220" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>218</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R220" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="221" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R221" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="222" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>220</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R222" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="223" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R223" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="224" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>222</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R224" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R225" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="226" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>224</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R226" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R227" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>226</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R228" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="229" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R229" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="230" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>228</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R230" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="231" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R231" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="232" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>230</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R232" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="233" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R233" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="234" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>232</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R234" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="235" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R235" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="236" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>234</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R236" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="237" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R237" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="238" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>236</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R238" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="239" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R239" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="240" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>238</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R240" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="241" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R241" s="9">
+        <v>3.4028234699999998E+38</v>
+      </c>
+    </row>
+    <row r="242" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>240</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R242" s="9"/>
+    </row>
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>252</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>254</v>
       </c>
@@ -5816,5 +7301,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>